<commit_message>
Refactor push-to-backstop logic and update furnace programs
Replaced specific PUSHTOBACKSTOP calls with parameterized version in LOAD_FURNACE.LS. Updated PICK_FURNACE1.LS to use new push distance register and removed inline calculation. Modified PUSHTOBACKSTOP.LS to set push distance based on argument and handle undefined cases. Updated registers_inputs_outputs.xlsx to reflect these changes.
</commit_message>
<xml_diff>
--- a/registers_inputs_outputs.xlsx
+++ b/registers_inputs_outputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
   <si>
     <t>Timer #</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>backoff_pshStrt</t>
+  </si>
+  <si>
+    <t>push_dist1</t>
+  </si>
+  <si>
+    <t>push_dist2</t>
   </si>
   <si>
     <t>zero90</t>
@@ -696,19 +702,19 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -716,16 +722,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -733,16 +739,16 @@
         <f>A2+1</f>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -750,14 +756,14 @@
         <f>A3+1</f>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -765,14 +771,14 @@
         <f>A4+1</f>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -780,14 +786,14 @@
         <f>A5+1</f>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -795,14 +801,14 @@
         <f>A6+1</f>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -810,14 +816,14 @@
         <f>A7+1</f>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -825,14 +831,14 @@
         <f>A8+1</f>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -840,14 +846,14 @@
         <f>A9+1</f>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
@@ -855,14 +861,14 @@
         <f>A10+1</f>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -870,14 +876,14 @@
         <f>A11+1</f>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -885,16 +891,16 @@
         <f>A12+1</f>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
@@ -902,14 +908,14 @@
         <f>A13+1</f>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -917,14 +923,14 @@
         <f>A14+1</f>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -932,14 +938,14 @@
         <f>A15+1</f>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -947,14 +953,14 @@
         <f>A16+1</f>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -962,14 +968,14 @@
         <f>A17+1</f>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -977,16 +983,16 @@
         <f>A18+1</f>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -994,16 +1000,16 @@
         <f>A19+1</f>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -1011,16 +1017,16 @@
         <f>A20+1</f>
       </c>
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -1028,16 +1034,16 @@
         <f>A21+1</f>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -1045,16 +1051,16 @@
         <f>A22+1</f>
       </c>
       <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -1062,16 +1068,16 @@
         <f>A23+1</f>
       </c>
       <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -1079,16 +1085,16 @@
         <f>A24+1</f>
       </c>
       <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
@@ -1096,16 +1102,16 @@
         <f>A25+1</f>
       </c>
       <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -1113,13 +1119,13 @@
         <f>A26+1</f>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1335,10 +1341,10 @@
         <f>A50+1</f>
       </c>
       <c r="B51" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1348,10 +1354,10 @@
         <f>A51+1</f>
       </c>
       <c r="B52" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1361,10 +1367,10 @@
         <f>A52+1</f>
       </c>
       <c r="B53" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1374,10 +1380,10 @@
         <f>A53+1</f>
       </c>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1387,10 +1393,10 @@
         <f>A54+1</f>
       </c>
       <c r="B55" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1400,10 +1406,10 @@
         <f>A55+1</f>
       </c>
       <c r="B56" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1629,10 +1635,10 @@
         <f>A80+1</f>
       </c>
       <c r="B81" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -1642,10 +1648,10 @@
         <f>A81+1</f>
       </c>
       <c r="B82" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -1655,10 +1661,10 @@
         <f>A82+1</f>
       </c>
       <c r="B83" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -1668,10 +1674,10 @@
         <f>A83+1</f>
       </c>
       <c r="B84" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -1681,10 +1687,10 @@
         <f>A84+1</f>
       </c>
       <c r="B85" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -1694,10 +1700,10 @@
         <f>A85+1</f>
       </c>
       <c r="B86" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3030,14 +3036,18 @@
       <c r="A31" s="3">
         <f>A30+1</f>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C31" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3">
         <f>A31+1</f>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C32" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
@@ -3514,7 +3524,7 @@
         <f>A99+1</f>
       </c>
       <c r="B100" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C100" s="2"/>
     </row>
@@ -3523,7 +3533,7 @@
         <f>A100+1</f>
       </c>
       <c r="B101" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C101" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fix syntax in conditional statements for push-to-backstop logic
</commit_message>
<xml_diff>
--- a/registers_inputs_outputs.xlsx
+++ b/registers_inputs_outputs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
   <si>
     <t>Timer #</t>
   </si>
@@ -129,7 +129,13 @@
     <t>push_dist1</t>
   </si>
   <si>
+    <t xml:space="preserve">push distance. calculated in pushtobackstop if AR[1]=1 </t>
+  </si>
+  <si>
     <t>push_dist2</t>
+  </si>
+  <si>
+    <t>push distance. calculated in pushtobackstop if AR[1]=2</t>
   </si>
   <si>
     <t>zero90</t>
@@ -702,19 +708,19 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -722,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -739,16 +745,16 @@
         <f>A2+1</f>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -756,14 +762,14 @@
         <f>A3+1</f>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -771,14 +777,14 @@
         <f>A4+1</f>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -786,14 +792,14 @@
         <f>A5+1</f>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -801,14 +807,14 @@
         <f>A6+1</f>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -816,14 +822,14 @@
         <f>A7+1</f>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -831,14 +837,14 @@
         <f>A8+1</f>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -846,14 +852,14 @@
         <f>A9+1</f>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
@@ -861,14 +867,14 @@
         <f>A10+1</f>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -876,14 +882,14 @@
         <f>A11+1</f>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -891,16 +897,16 @@
         <f>A12+1</f>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
@@ -908,14 +914,14 @@
         <f>A13+1</f>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -923,14 +929,14 @@
         <f>A14+1</f>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -938,14 +944,14 @@
         <f>A15+1</f>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -953,14 +959,14 @@
         <f>A16+1</f>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -968,14 +974,14 @@
         <f>A17+1</f>
       </c>
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -983,16 +989,16 @@
         <f>A18+1</f>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -1000,16 +1006,16 @@
         <f>A19+1</f>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -1017,16 +1023,16 @@
         <f>A20+1</f>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -1034,16 +1040,16 @@
         <f>A21+1</f>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -1051,16 +1057,16 @@
         <f>A22+1</f>
       </c>
       <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -1068,16 +1074,16 @@
         <f>A23+1</f>
       </c>
       <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -1085,16 +1091,16 @@
         <f>A24+1</f>
       </c>
       <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
@@ -1102,16 +1108,16 @@
         <f>A25+1</f>
       </c>
       <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -1119,13 +1125,13 @@
         <f>A26+1</f>
       </c>
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -1341,10 +1347,10 @@
         <f>A50+1</f>
       </c>
       <c r="B51" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1354,10 +1360,10 @@
         <f>A51+1</f>
       </c>
       <c r="B52" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1367,10 +1373,10 @@
         <f>A52+1</f>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1380,10 +1386,10 @@
         <f>A53+1</f>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1393,10 +1399,10 @@
         <f>A54+1</f>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1406,10 +1412,10 @@
         <f>A55+1</f>
       </c>
       <c r="B56" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1635,10 +1641,10 @@
         <f>A80+1</f>
       </c>
       <c r="B81" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -1648,10 +1654,10 @@
         <f>A81+1</f>
       </c>
       <c r="B82" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -1661,10 +1667,10 @@
         <f>A82+1</f>
       </c>
       <c r="B83" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -1674,10 +1680,10 @@
         <f>A83+1</f>
       </c>
       <c r="B84" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -1687,10 +1693,10 @@
         <f>A84+1</f>
       </c>
       <c r="B85" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -1700,10 +1706,10 @@
         <f>A85+1</f>
       </c>
       <c r="B86" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3039,16 +3045,20 @@
       <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3">
         <f>A31+1</f>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3">
@@ -3524,7 +3534,7 @@
         <f>A99+1</f>
       </c>
       <c r="B100" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C100" s="2"/>
     </row>
@@ -3533,7 +3543,7 @@
         <f>A100+1</f>
       </c>
       <c r="B101" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C101" s="2"/>
     </row>

</xml_diff>